<commit_message>
Ultimos cambios de Empeños
Cambios finales
</commit_message>
<xml_diff>
--- a/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteVencidos.xlsx
+++ b/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteVencidos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Empe-o\Empeño.WindowsForms\Empeños\Comprobantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtjarquinm\Documents\GitHub-Donovan\Empe-o\Empeño.WindowsForms\Empeños\Comprobantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE6EF20-08AE-4D4F-BA33-BA79048AA312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3948" windowWidth="28800" windowHeight="15456"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -104,10 +105,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -191,9 +192,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -206,7 +207,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -222,9 +223,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -239,7 +243,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -531,101 +535,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.44140625" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
     <col min="2" max="2" width="99" customWidth="1"/>
-    <col min="3" max="3" width="32.88671875" customWidth="1"/>
-    <col min="4" max="4" width="67.88671875" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" ht="64.95" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A2" s="16" t="s">
+    <row r="1" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-    </row>
-    <row r="3" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A5" s="16" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A7" s="16" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A8" s="9"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A8" s="11"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:8" ht="52.2" customHeight="1" x14ac:dyDescent="0.95">
+    <row r="9" spans="1:8" ht="52.15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -633,15 +637,15 @@
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -655,142 +659,142 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A18" s="11" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A19" s="11" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A20" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-    </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="21" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+    </row>
+    <row r="22" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A22" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A23" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+    <row r="25" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A26" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-    </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+    </row>
+    <row r="27" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-    </row>
-    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A29" s="14" t="s">
+    <row r="28" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A29" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-    </row>
-    <row r="31" spans="1:4" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-    </row>
-    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A32" s="13" t="s">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A32" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>